<commit_message>
NVDA update, TSM new model
</commit_message>
<xml_diff>
--- a/HardwareSemis.xlsx
+++ b/HardwareSemis.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFFCB6B-F049-4088-BE2C-DFB377DB6CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D2C71D-D173-4EF0-B1BE-5F12CE3B0CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26775" yWindow="2010" windowWidth="23250" windowHeight="18870" xr2:uid="{98D8347A-DFA4-427C-8784-96E5573B433C}"/>
+    <workbookView xWindow="-30465" yWindow="975" windowWidth="30015" windowHeight="18480" xr2:uid="{98D8347A-DFA4-427C-8784-96E5573B433C}"/>
   </bookViews>
   <sheets>
     <sheet name="Semiconductors" sheetId="1" r:id="rId1"/>
     <sheet name="Networking" sheetId="3" r:id="rId2"/>
     <sheet name="Electronics-Computers" sheetId="2" r:id="rId3"/>
+    <sheet name="FX" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -413,6 +416,12 @@
   </si>
   <si>
     <t>Q224</t>
+  </si>
+  <si>
+    <t>Q124</t>
+  </si>
+  <si>
+    <t>NTD/TWD</t>
   </si>
 </sst>
 </file>
@@ -521,26 +530,28 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Quarterly Earnings Preview"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="K3">
-            <v>2460</v>
+            <v>24600</v>
           </cell>
         </row>
         <row r="5">
           <cell r="K5">
-            <v>13143</v>
+            <v>31438</v>
           </cell>
         </row>
         <row r="6">
           <cell r="K6">
-            <v>10950</v>
+            <v>9710</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -608,7 +619,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -643,8 +654,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -697,6 +708,74 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="J4">
+            <v>25931</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="J7">
+            <v>67370</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>30421</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>4800</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>11864</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>73468</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1005,7 +1084,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1013,7 +1092,11 @@
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="9" width="9.140625" style="3"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="3"/>
     <col min="10" max="10" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1060,29 +1143,29 @@
         <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>266.69</v>
+        <v>120</v>
       </c>
       <c r="E3" s="6">
         <f>+D3*H3</f>
-        <v>656057.4</v>
+        <v>2952000</v>
       </c>
       <c r="F3" s="6">
         <f>+[1]Main!$K$5-[1]Main!$K$6</f>
-        <v>2193</v>
+        <v>21728</v>
       </c>
       <c r="G3" s="6">
         <f>+E3-F3</f>
-        <v>653864.4</v>
+        <v>2930272</v>
       </c>
       <c r="H3" s="6">
         <f>+[1]Main!$K$3</f>
-        <v>2460</v>
+        <v>24600</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="J3" s="10">
-        <v>44937</v>
+        <v>45532</v>
       </c>
       <c r="K3">
         <v>1993</v>
@@ -1092,23 +1175,73 @@
       <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="4">
+        <v>169</v>
+      </c>
+      <c r="E4" s="6">
+        <f>+D4*H4/5</f>
+        <v>876467.8</v>
+      </c>
+      <c r="F4" s="6">
+        <f>+[6]Main!$J$7-[6]Main!$J$8</f>
+        <v>36949</v>
+      </c>
+      <c r="G4" s="6">
+        <f>+E4-F4</f>
+        <v>839518.8</v>
+      </c>
+      <c r="H4" s="6">
+        <f>+[6]Main!$J$4</f>
+        <v>25931</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="10">
+        <v>45532</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
+      <c r="D5" s="4">
+        <v>964</v>
+      </c>
+      <c r="E5" s="6">
+        <f>+D5*H5/FX!C2</f>
+        <v>781904.41038473567</v>
+      </c>
+      <c r="F5" s="6">
+        <f>+[6]Main!$J$7-[6]Main!$J$8</f>
+        <v>36949</v>
+      </c>
+      <c r="G5" s="6">
+        <f>+E5-F5</f>
+        <v>744955.41038473567</v>
+      </c>
+      <c r="H5" s="6">
+        <f>+[6]Main!$J$4</f>
+        <v>25931</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" s="10">
+        <v>45532</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1125,12 +1258,34 @@
       <c r="A7" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
+      <c r="D7" s="4">
+        <v>154</v>
+      </c>
+      <c r="E7" s="6">
+        <f>+D7*H7</f>
+        <v>739200</v>
+      </c>
+      <c r="F7" s="6">
+        <f>+[7]Main!$J$5-[7]Main!$J$6</f>
+        <v>-61604</v>
+      </c>
+      <c r="G7" s="6">
+        <f>+E7-F7</f>
+        <v>800804</v>
+      </c>
+      <c r="H7" s="6">
+        <f>+[7]Main!$J$3</f>
+        <v>4800</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1159,74 +1314,74 @@
         <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3">
-        <v>170.34</v>
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
+        <v>130</v>
       </c>
       <c r="E10" s="6">
         <f>+D10*H10</f>
+        <v>210340</v>
+      </c>
+      <c r="F10" s="6">
+        <f>+[3]Main!$M$5-[3]Main!$M$6</f>
+        <v>3388</v>
+      </c>
+      <c r="G10" s="6">
+        <f>+E10-F10</f>
+        <v>206952</v>
+      </c>
+      <c r="H10" s="6">
+        <f>+[3]Main!$M$3</f>
+        <v>1618</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="10">
+        <v>45507</v>
+      </c>
+      <c r="K10">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <v>170.34</v>
+      </c>
+      <c r="E11" s="6">
+        <f>+D11*H11</f>
         <v>154595.76542208</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F11" s="6">
         <f>+[2]Main!$K$5-[2]Main!$K$6</f>
         <v>1153</v>
       </c>
-      <c r="G10" s="6">
-        <f>+E10-F10</f>
+      <c r="G11" s="6">
+        <f>+E11-F11</f>
         <v>153442.76542208</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H11" s="6">
         <f>+[2]Main!$K$3</f>
         <v>907.57171200000005</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J11" s="10">
         <v>44946</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4">
-        <v>130</v>
-      </c>
-      <c r="E11" s="6">
-        <f>+D11*H11</f>
-        <v>210340</v>
-      </c>
-      <c r="F11" s="6">
-        <f>+[3]Main!$M$5-[3]Main!$M$6</f>
-        <v>3388</v>
-      </c>
-      <c r="G11" s="6">
-        <f>+E11-F11</f>
-        <v>206952</v>
-      </c>
-      <c r="H11" s="6">
-        <f>+[3]Main!$M$3</f>
-        <v>1618</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" s="10">
-        <v>45507</v>
-      </c>
-      <c r="K11">
-        <v>1969</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1503,9 +1658,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{82B60337-F6F7-4A89-BE21-94E4E4FAE923}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{89BFBE39-15FE-4D88-BD35-419556A195F8}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{89BFBE39-15FE-4D88-BD35-419556A195F8}"/>
     <hyperlink ref="B12" r:id="rId3" xr:uid="{ACBF0F19-D83E-41D4-B3AD-01439A0CCE2D}"/>
-    <hyperlink ref="B11" r:id="rId4" xr:uid="{0B4AADBB-7802-4155-9477-7B8867856D77}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{0B4AADBB-7802-4155-9477-7B8867856D77}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{D5C26AF1-ADC4-4E03-9D8B-12F3C24C324B}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{DD4F0CC9-D485-4053-9B41-DE6F39511946}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{05815C98-BE17-4CF3-942D-C5BFAB80DA80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1949,4 +2107,30 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC72FDEE-60E0-4B9B-AACF-AB184FD947A1}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2">
+        <v>31.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>